<commit_message>
Added alot of stuff
</commit_message>
<xml_diff>
--- a/application/reports/Report.xlsx
+++ b/application/reports/Report.xlsx
@@ -6,7 +6,7 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Test" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -14,15 +14,93 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
-  <si>
-    <t>Row1</t>
-  </si>
-  <si>
-    <t>Row2</t>
-  </si>
-  <si>
-    <t>Row3</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
+  <si>
+    <t>Building</t>
+  </si>
+  <si>
+    <t>Floor</t>
+  </si>
+  <si>
+    <t>Room</t>
+  </si>
+  <si>
+    <t>Storage</t>
+  </si>
+  <si>
+    <t>Barcode</t>
+  </si>
+  <si>
+    <t>Chemical Name</t>
+  </si>
+  <si>
+    <t>Current Quantity</t>
+  </si>
+  <si>
+    <t>Current Unit</t>
+  </si>
+  <si>
+    <t>Science</t>
+  </si>
+  <si>
+    <t>Basement</t>
+  </si>
+  <si>
+    <t>13A</t>
+  </si>
+  <si>
+    <t>E1-3299</t>
+  </si>
+  <si>
+    <t>PHOSPHATE</t>
+  </si>
+  <si>
+    <t>gram (g)</t>
+  </si>
+  <si>
+    <t>N1-15</t>
+  </si>
+  <si>
+    <t>2-CHLOROBUTANE</t>
+  </si>
+  <si>
+    <t>17040000</t>
+  </si>
+  <si>
+    <t>2,6-DICHLOROINDOPHENOL SODIUM DERIVATIVE</t>
+  </si>
+  <si>
+    <t>Cyanide Cabinet</t>
+  </si>
+  <si>
+    <t>E1-3399</t>
+  </si>
+  <si>
+    <t>2-(DIMETHYLAMINO)PYRIDINE</t>
+  </si>
+  <si>
+    <t>13C</t>
+  </si>
+  <si>
+    <t>E1-3540</t>
+  </si>
+  <si>
+    <t>2-BROMOBUTANE</t>
+  </si>
+  <si>
+    <t>16020008</t>
+  </si>
+  <si>
+    <t>ACETIC ACID 99+%</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>203</t>
+  </si>
+  <si>
+    <t>D1-8364</t>
   </si>
 </sst>
 </file>
@@ -358,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -366,7 +444,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -375,6 +453,203 @@
       </c>
       <c r="C1" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="n">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="n">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="n">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="n">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="n">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" t="n">
+        <v>33</v>
+      </c>
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="n">
+        <v>22</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the Report Query
</commit_message>
<xml_diff>
--- a/application/reports/Report.xlsx
+++ b/application/reports/Report.xlsx
@@ -64,43 +64,43 @@
     <t>2-CHLOROBUTANE</t>
   </si>
   <si>
+    <t>Cyanide Cabinet</t>
+  </si>
+  <si>
+    <t>E1-3399</t>
+  </si>
+  <si>
+    <t>2-(DIMETHYLAMINO)PYRIDINE</t>
+  </si>
+  <si>
+    <t>13C</t>
+  </si>
+  <si>
+    <t>E1-3540</t>
+  </si>
+  <si>
+    <t>2-BROMOBUTANE</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>203</t>
+  </si>
+  <si>
+    <t>D1-8364</t>
+  </si>
+  <si>
+    <t>2,6-DICHLOROINDOPHENOL SODIUM DERIVATIVE</t>
+  </si>
+  <si>
     <t>17040000</t>
   </si>
   <si>
-    <t>2,6-DICHLOROINDOPHENOL SODIUM DERIVATIVE</t>
-  </si>
-  <si>
-    <t>Cyanide Cabinet</t>
-  </si>
-  <si>
-    <t>E1-3399</t>
-  </si>
-  <si>
-    <t>2-(DIMETHYLAMINO)PYRIDINE</t>
-  </si>
-  <si>
-    <t>13C</t>
-  </si>
-  <si>
-    <t>E1-3540</t>
-  </si>
-  <si>
-    <t>2-BROMOBUTANE</t>
-  </si>
-  <si>
     <t>16020008</t>
   </si>
   <si>
     <t>ACETIC ACID 99+%</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>203</t>
-  </si>
-  <si>
-    <t>D1-8364</t>
   </si>
 </sst>
 </file>
@@ -533,16 +533,16 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G4" t="n">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="H4" t="s">
         <v>13</v>
@@ -556,16 +556,16 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G5" t="n">
         <v>22</v>
@@ -579,19 +579,19 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G6" t="n">
         <v>22</v>
@@ -608,13 +608,13 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
         <v>25</v>
@@ -631,22 +631,22 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
         <v>27</v>
       </c>
-      <c r="D8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>28</v>
       </c>
-      <c r="F8" t="s">
-        <v>17</v>
-      </c>
       <c r="G8" t="n">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="H8" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Added in more report functionality
</commit_message>
<xml_diff>
--- a/application/reports/Report.xlsx
+++ b/application/reports/Report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
   <si>
     <t>Building</t>
   </si>
@@ -40,67 +40,22 @@
     <t>Current Unit</t>
   </si>
   <si>
-    <t>Science</t>
+    <t>Frost</t>
   </si>
   <si>
     <t>Basement</t>
   </si>
   <si>
-    <t>13A</t>
-  </si>
-  <si>
-    <t>E1-3299</t>
-  </si>
-  <si>
-    <t>PHOSPHATE</t>
+    <t>04</t>
+  </si>
+  <si>
+    <t>E1-3399</t>
+  </si>
+  <si>
+    <t>2-(DIMETHYLAMINO)PYRIDINE</t>
   </si>
   <si>
     <t>gram (g)</t>
-  </si>
-  <si>
-    <t>N1-15</t>
-  </si>
-  <si>
-    <t>2-CHLOROBUTANE</t>
-  </si>
-  <si>
-    <t>Cyanide Cabinet</t>
-  </si>
-  <si>
-    <t>E1-3399</t>
-  </si>
-  <si>
-    <t>2-(DIMETHYLAMINO)PYRIDINE</t>
-  </si>
-  <si>
-    <t>13C</t>
-  </si>
-  <si>
-    <t>E1-3540</t>
-  </si>
-  <si>
-    <t>2-BROMOBUTANE</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>203</t>
-  </si>
-  <si>
-    <t>D1-8364</t>
-  </si>
-  <si>
-    <t>2,6-DICHLOROINDOPHENOL SODIUM DERIVATIVE</t>
-  </si>
-  <si>
-    <t>17040000</t>
-  </si>
-  <si>
-    <t>16020008</t>
-  </si>
-  <si>
-    <t>ACETIC ACID 99+%</t>
   </si>
 </sst>
 </file>
@@ -436,7 +391,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,165 +445,9 @@
         <v>12</v>
       </c>
       <c r="G2" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="n">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="n">
-        <v>22</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" t="n">
-        <v>22</v>
-      </c>
-      <c r="H5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" t="n">
-        <v>22</v>
-      </c>
-      <c r="H6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" t="n">
-        <v>33</v>
-      </c>
-      <c r="H7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" t="n">
-        <v>33</v>
-      </c>
-      <c r="H8" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added ability to report by hazard
</commit_message>
<xml_diff>
--- a/application/reports/Report.xlsx
+++ b/application/reports/Report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <t>Building</t>
   </si>
@@ -40,22 +40,46 @@
     <t>Current Unit</t>
   </si>
   <si>
-    <t>Frost</t>
+    <t>Primary Hazard</t>
+  </si>
+  <si>
+    <t>Science</t>
   </si>
   <si>
     <t>Basement</t>
   </si>
   <si>
-    <t>04</t>
-  </si>
-  <si>
-    <t>E1-3399</t>
-  </si>
-  <si>
-    <t>2-(DIMETHYLAMINO)PYRIDINE</t>
+    <t>13C</t>
+  </si>
+  <si>
+    <t>17050002</t>
+  </si>
+  <si>
+    <t>BASE CHEMICAL</t>
   </si>
   <si>
     <t>gram (g)</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>17050007</t>
+  </si>
+  <si>
+    <t>OXIDIZER CHEMICAL</t>
+  </si>
+  <si>
+    <t>Oxidizer</t>
+  </si>
+  <si>
+    <t>17050008</t>
+  </si>
+  <si>
+    <t>REACTIVE CHEMICAL</t>
+  </si>
+  <si>
+    <t>Reactive</t>
   </si>
 </sst>
 </file>
@@ -391,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -399,7 +423,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,31 +448,95 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="n">
+        <v>3223</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="n">
+        <v>33</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="n">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="n">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>